<commit_message>
worked on wrong word issue
</commit_message>
<xml_diff>
--- a/Final/test.xlsx
+++ b/Final/test.xlsx
@@ -403,7 +403,7 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData/>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
@@ -418,13 +418,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A8" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A22" xSplit="0" ySplit="1"/>
+      <selection activeCell="A8" activeCellId="0" pane="topLeft" sqref="A8"/>
+      <selection activeCell="A34" activeCellId="0" pane="bottomLeft" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
     <row customFormat="1" customHeight="1" ht="13.8" r="1" s="3">
       <c r="A1" s="3" t="inlineStr">
@@ -437,6 +439,11 @@
           <t>Definition</t>
         </is>
       </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Pronunciation</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="2" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -449,6 +456,11 @@
           <t>a series of columns set at regular intervals and usually supporting the base of a roof structure</t>
         </is>
       </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>ˌkä-lə-ˈnād</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="3" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -461,6 +473,11 @@
           <t>a moderate red</t>
         </is>
       </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>sə-ˈrēs</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="4" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -473,6 +490,11 @@
           <t>to cut transversely</t>
         </is>
       </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>tran(t)-ˈsekt</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="5" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -485,6 +507,11 @@
           <t>a heavy substance (such as rocks or water) placed in such a way as to improve stability and control (as of the draft of a ship or the buoyancy of a balloon or submarine)</t>
         </is>
       </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>ˈba-ləst</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="6" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -497,6 +524,11 @@
           <t>characterized by harsh, insistent, and discordant sound; also : commanding attention by a loud or obtrusive quality</t>
         </is>
       </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>ˈstrī-dᵊnt</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="7" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -509,6 +541,11 @@
           <t>an act, process, or instance of transposing or being transposed</t>
         </is>
       </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>ˌtran(t)s-pə-ˈzi-shən</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="8" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -521,6 +558,11 @@
           <t>the use of a speech form that lacks a final or initial sound which a variant speech form has (such as 's instead of is in there's)</t>
         </is>
       </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>i-ˈli-zhən</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="9" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -533,6 +575,11 @@
           <t>an auxiliary proposition used in the demonstration of another proposition</t>
         </is>
       </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>ˈle-mə</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="10" s="4">
       <c r="A10" s="5" t="inlineStr">
@@ -543,6 +590,419 @@
       <c r="B10" s="5" t="inlineStr">
         <is>
           <t>having or showing skill, cleverness, or resourcefulness in handling situations</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>ə-ˈdrȯit</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="11" s="4">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>transverse</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>acting, lying, or being across : set crosswise</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>tran(t)s-ˈvərs</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="12" s="4">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>proposition</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>something offered for consideration or acceptance : proposal</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>ˌprä-pə-ˈzi-shən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="13" s="4">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>anagoge</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>interpretation of a word, passage, or text (as of Scripture or poetry) that finds beyond the literal, allegorical, and moral senses a fourth and ultimate spiritual or mystical sense</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>ˈa-nə-ˌgō-jē</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="14" s="4">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>languor</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>weakness or weariness of body or mind</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>ˈlaŋ-gər</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="15" s="4">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>patina</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>a usually green film formed naturally on copper and bronze by long exposure or artificially (as by acids) and often valued aesthetically for its color</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>pə-ˈtē-nə</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="16" s="4">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>concupiscence</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>strong desire; especially : sexual desire</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>kän-ˈkyü-pə-sən(t)s</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="17" s="4">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>ardent</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>characterized by warmth of feeling typically expressed in eager zealous support or activity</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>ˈär-dᵊnt</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="18" s="4">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>despondent</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>feeling or showing extreme discouragement, dejection, or depression</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>di-ˈspän-dənt</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="19" s="4">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>bravura</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>a musical passage requiring exceptional agility and technical skill in execution</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>brə-ˈvyu̇r-ə</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="4">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>rubicund</t>
+        </is>
+      </c>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>ruddy</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t>ˈrü-bi-(ˌ)kənd</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="4">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>maladroitly</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>lacking adroitness : inept</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>ˌma-lə-ˈdrȯit</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="4">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>affable</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>being pleasant and at ease in talking to others</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>ˈa-fə-bəl</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="4">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>nonchalance</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>the quality or state of being nonchalant</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>ˌnän-shə-ˈlän(t)s</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="4">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>dormition</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>death resembling falling asleep</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>dȯrˈmishən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="25" s="4">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>sagacious</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>of keen and farsighted penetration and judgment : discerning</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sə-ˈgā-shəs</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="26" s="4">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>vigil</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="inlineStr">
+        <is>
+          <t>the act of keeping awake at times when sleep is customary; also : a period of wakefulness</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="inlineStr">
+        <is>
+          <t>ˈvi-jəl</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="27" s="4">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>retinue</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>a group of retainers or attendants</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>ˈre-tə-ˌnü</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="28" s="4">
+      <c r="A28" s="5" t="inlineStr">
+        <is>
+          <t>inviolate</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="inlineStr">
+        <is>
+          <t>not violated or profaned; especially : pure</t>
+        </is>
+      </c>
+      <c r="C28" s="5" t="inlineStr">
+        <is>
+          <t>(ˌ)in-ˈvī-ə-lət</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="29" s="4">
+      <c r="A29" s="5" t="inlineStr">
+        <is>
+          <t>attenuation</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="inlineStr">
+        <is>
+          <t>the act or process of attenuating something or the state of being attenuated: such as</t>
+        </is>
+      </c>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>ə-ˌten-yə-ˈwā-shən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="30" s="4">
+      <c r="A30" s="5" t="inlineStr">
+        <is>
+          <t>ratiocination</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="inlineStr">
+        <is>
+          <t>the process of exact thinking : reasoning</t>
+        </is>
+      </c>
+      <c r="C30" s="5" t="inlineStr">
+        <is>
+          <t>ˌra-tē-ˌō-sə-ˈnā-shən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="31" s="4">
+      <c r="A31" s="5" t="inlineStr">
+        <is>
+          <t>enstatsis</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="C31" s="5" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="32" s="4">
+      <c r="A32" s="5" t="inlineStr">
+        <is>
+          <t>concomitant</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="inlineStr">
+        <is>
+          <t>accompanying especially in a subordinate or incidental way</t>
+        </is>
+      </c>
+      <c r="C32" s="5" t="inlineStr">
+        <is>
+          <t>kən-ˈkä-mə-tənt</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="33" s="4">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
+          <t>foo</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="inlineStr">
+        <is>
+          <t>a mythical lion-dog used as a decorative motif in Far Eastern art</t>
+        </is>
+      </c>
+      <c r="C33" s="5" t="inlineStr">
+        <is>
+          <t>ˈfü-</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="34" s="4">
+      <c r="A34" s="5" t="inlineStr">
+        <is>
+          <t>tine</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>a slender pointed projecting part : prong</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ˈtīn</t>
         </is>
       </c>
     </row>
@@ -565,7 +1025,7 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData/>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
@@ -586,7 +1046,7 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData/>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
used hwi to fix bug
</commit_message>
<xml_diff>
--- a/Final/test.xlsx
+++ b/Final/test.xlsx
@@ -2366,6 +2366,11 @@
           <t>of, relating to, or being water or solutions in the earth's crust above the permanent groundwater level</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ˈvā-ˌdōs</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="4" s="5">
       <c r="A4" s="6" t="inlineStr">
@@ -2390,6 +2395,11 @@
           <t>a written agreement between belligerent nations</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>kär-ˈtel</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="6" s="5">
       <c r="A6" s="6" t="inlineStr">
@@ -2409,6 +2419,11 @@
           <t>a usually rhetorical break in the flow of sound in the middle of a line of verse</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>si-ˈzyu̇r-ə</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="8" s="5">
       <c r="A8" s="6" t="inlineStr">
@@ -2442,6 +2457,11 @@
           <t>discreetly cautious: such as</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ˈcher-ē</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="12" s="5">
       <c r="A12" s="6" t="inlineStr">
@@ -2485,6 +2505,11 @@
           <t>a pottery fragment usually unearthed as an archaeological relic</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ˈpät-ˌshərd</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="16" s="5">
       <c r="A16" s="6" t="inlineStr">
@@ -2497,6 +2522,11 @@
           <t>a rapid whirling about of the body; especially : a full turn on the toe or ball of one foot in ballet</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ˌpir-ə-ˈwet</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="17" s="5">
       <c r="A17" s="6" t="inlineStr">
@@ -2547,6 +2577,11 @@
           <t>frothy matter on liquids : foam, scum</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ˈspyüm</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="22" s="5">
       <c r="A22" s="6" t="inlineStr">
@@ -2559,6 +2594,11 @@
           <t>a filling thread or yarn in weaving</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ˈweft</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="23" s="5">
       <c r="A23" s="6" t="inlineStr">
@@ -2571,6 +2611,11 @@
           <t>a raw hide soaked in lye to remove the hair and dried</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ˈpär-ˌflesh</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="24" s="5">
       <c r="A24" s="6" t="inlineStr">
@@ -2597,6 +2642,11 @@
           <t>the capacity for or the act of forming or entertaining ideas</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ˌī-dē-ˈā-shən</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="27" s="5">
       <c r="A27" s="6" t="inlineStr">
@@ -2621,6 +2671,11 @@
           <t>a person dressed in ragged clothing : ragamuffin</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ˌta-tər-di-ˈmāl-yən</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="29" s="5">
       <c r="A29" s="6" t="inlineStr">
@@ -2633,6 +2688,11 @@
           <t>skiing in a zigzag or wavy course between upright obstacles (such as flags)</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ˈslä-ləm</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="30" s="5">
       <c r="A30" s="6" t="inlineStr">
@@ -2652,6 +2712,11 @@
           <t>a low-lying or depressed and often wet stretch of land; also : a shallow depression on a golf course</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ˈswāl</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="32" s="5">
       <c r="A32" s="6" t="inlineStr">
@@ -2664,6 +2729,11 @@
           <t>a steep slope in front of a fortification</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>i-ˈskärp-mənt</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="33" s="5">
       <c r="A33" s="6" t="inlineStr">
@@ -2683,9 +2753,14 @@
           <t>euchre</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="6" t="inlineStr">
         <is>
           <t>a card game in which each player is dealt five cards and the player making trump must take three tricks to win a hand</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ˈyü-kər</t>
         </is>
       </c>
     </row>
@@ -2702,9 +2777,14 @@
           <t>armature</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="6" t="inlineStr">
         <is>
           <t>an organ or structure (such as teeth or thorns) for offense or defense</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ˈär-mə-ˌchu̇r</t>
         </is>
       </c>
     </row>
@@ -2721,9 +2801,14 @@
           <t>cravat</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="6" t="inlineStr">
         <is>
           <t>a band or scarf worn around the neck</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>krə-ˈvat</t>
         </is>
       </c>
     </row>
@@ -2733,9 +2818,14 @@
           <t>shoat</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="6" t="inlineStr">
         <is>
           <t>a young hog and especially one that has been weaned</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ˈshōt</t>
         </is>
       </c>
     </row>
@@ -2745,9 +2835,14 @@
           <t>cartouche</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="6" t="inlineStr">
         <is>
           <t>a gun cartridge with a paper case</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>kär-ˈtüsh</t>
         </is>
       </c>
     </row>
@@ -2757,7 +2852,7 @@
           <t>debouched</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="6" t="inlineStr">
         <is>
           <t>to cause to emerge : discharge</t>
         </is>
@@ -2769,9 +2864,14 @@
           <t>crenellated</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="6" t="inlineStr">
         <is>
           <t>having crenellations</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ˈkre-nə-ˌlā-təd</t>
         </is>
       </c>
     </row>
@@ -2788,6 +2888,16 @@
           <t>argosy</t>
         </is>
       </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>a large ship; especially : a large merchant ship</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ˈär-gə-sē</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="45" s="5">
       <c r="A45" s="6" t="inlineStr">
@@ -2795,6 +2905,16 @@
           <t>sloe</t>
         </is>
       </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>the small dark globose astringent fruit of the blackthorn; also : blackthorn</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ˈslō</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="46" s="5">
       <c r="A46" s="6" t="inlineStr">
@@ -2823,11 +2943,31 @@
           <t>pulque</t>
         </is>
       </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>a Mexican alcoholic beverage made from the fermented sap of various agaves (such as Agave atrovirens)</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ˈpül-ˌkā</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="50" s="5">
       <c r="A50" s="6" t="inlineStr">
         <is>
           <t>charivari</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>shivaree</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ˌshi-və-ˈrē</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
figured it out, word was not self.word
</commit_message>
<xml_diff>
--- a/Final/test.xlsx
+++ b/Final/test.xlsx
@@ -421,7 +421,7 @@
       <selection activeCell="A124" activeCellId="0" pane="bottomLeft" sqref="A124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.921875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.95703125" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
     <row customFormat="1" customHeight="1" ht="13.8" r="1" s="4">
       <c r="A1" s="4" t="inlineStr">
@@ -2326,10 +2326,10 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A8" view="normal" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="A34" activeCellId="0" pane="topLeft" sqref="A34"/>
+      <selection activeCell="A47" activeCellId="0" pane="topLeft" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.921875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.95703125" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
     <row customFormat="1" customHeight="1" ht="13.8" r="1" s="7">
       <c r="A1" s="7" t="inlineStr">
@@ -2351,575 +2351,635 @@
     <row customHeight="1" ht="15" r="2" s="5">
       <c r="A2" s="6" t="inlineStr">
         <is>
-          <t>legflung</t>
+          <t>quirting</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>a riding whip with a short handle and a rawhide lash</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ˈkwərt</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="3" s="5">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>vadose</t>
+          <t>supernumeraries</t>
         </is>
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>of, relating to, or being water or solutions in the earth's crust above the permanent groundwater level</t>
+          <t>exceeding the usual, stated, or prescribed number</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ˈvā-ˌdōs</t>
+          <t>ˌsü-pər-ˈnü-mə-ˌrer-ē</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="4" s="5">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>larval</t>
-        </is>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>the immature, wingless, and often wormlike feeding form that hatches from the egg of many insects, alters chiefly in size while passing through several molts, and is finally transformed into a pupa or chrysalis from which the adult emerges</t>
+          <t>legflung</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="5" s="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>cartel</t>
+          <t>vadose</t>
         </is>
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>a written agreement between belligerent nations</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>kär-ˈtel</t>
+          <t>of, relating to, or being water or solutions in the earth's crust above the permanent groundwater level</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>ˈvā-ˌdōs</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="6" s="5">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>carreta</t>
+          <t>larval</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>the immature, wingless, and often wormlike feeding form that hatches from the egg of many insects, alters chiefly in size while passing through several molts, and is finally transformed into a pupa or chrysalis from which the adult emerges</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>ˈlär-və</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="7" s="5">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>caesura</t>
+          <t>cartel</t>
         </is>
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>a usually rhetorical break in the flow of sound in the middle of a line of verse</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>si-ˈzyu̇r-ə</t>
+          <t>a written agreement between belligerent nations</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>kär-ˈtel</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="8" s="5">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>robozos</t>
+          <t>carreta</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="9" s="5">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>alqunogre</t>
+          <t>caesura</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>a usually rhetorical break in the flow of sound in the middle of a line of verse</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t>si-ˈzyu̇r-ə</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="10" s="5">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>calabozo</t>
+          <t>robozos</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="11" s="5">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>chary</t>
-        </is>
-      </c>
-      <c r="B11" s="6" t="inlineStr">
-        <is>
-          <t>discreetly cautious: such as</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>ˈcher-ē</t>
+          <t>alqunogre</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="12" s="5">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>heliotropic</t>
-        </is>
-      </c>
-      <c r="B12" s="6" t="inlineStr">
-        <is>
-          <t>phototropism in which sunlight is the orienting stimulus</t>
+          <t>calabozo</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="13" s="5">
       <c r="A13" s="6" t="inlineStr">
         <is>
-          <t>mullioned</t>
+          <t>chary</t>
         </is>
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>a slender vertical member that forms a division between units of a window, door, or screen or is used decoratively</t>
+          <t>discreetly cautious: such as</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>ˈcher-ē</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="14" s="5">
       <c r="A14" s="6" t="inlineStr">
         <is>
-          <t>garrafa</t>
+          <t>heliotropic</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>phototropism in which sunlight is the orienting stimulus</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>ˌhē-lē-ˈä-trə-ˌpi-zəm</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="15" s="5">
       <c r="A15" s="6" t="inlineStr">
         <is>
-          <t>potsherd</t>
+          <t>mullioned</t>
         </is>
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
-          <t>a pottery fragment usually unearthed as an archaeological relic</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ˈpät-ˌshərd</t>
+          <t>a slender vertical member that forms a division between units of a window, door, or screen or is used decoratively</t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>ˈməl-yən</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="16" s="5">
       <c r="A16" s="6" t="inlineStr">
         <is>
-          <t>pirouette</t>
-        </is>
-      </c>
-      <c r="B16" s="6" t="inlineStr">
-        <is>
-          <t>a rapid whirling about of the body; especially : a full turn on the toe or ball of one foot in ballet</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ˌpir-ə-ˈwet</t>
+          <t>garrafa</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="17" s="5">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>ossature</t>
+          <t>potsherd</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>a pottery fragment usually unearthed as an archaeological relic</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="inlineStr">
+        <is>
+          <t>ˈpät-ˌshərd</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="18" s="5">
       <c r="A18" s="6" t="inlineStr">
         <is>
-          <t>arraigned</t>
+          <t>pirouette</t>
         </is>
       </c>
       <c r="B18" s="6" t="inlineStr">
         <is>
-          <t>to call (a defendant) before a court to answer to an indictment : charge</t>
+          <t>a rapid whirling about of the body; especially : a full turn on the toe or ball of one foot in ballet</t>
+        </is>
+      </c>
+      <c r="C18" s="6" t="inlineStr">
+        <is>
+          <t>ˌpir-ə-ˈwet</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="19" s="5">
       <c r="A19" s="6" t="inlineStr">
         <is>
-          <t>querent</t>
+          <t>ossature</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="20" s="5">
       <c r="A20" s="6" t="inlineStr">
         <is>
-          <t>riffled</t>
+          <t>arraigned</t>
         </is>
       </c>
       <c r="B20" s="6" t="inlineStr">
         <is>
-          <t>to form, flow over, or move in riffles</t>
+          <t>to call (a defendant) before a court to answer to an indictment : charge</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>ə-ˈrān</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="21" s="5">
       <c r="A21" s="6" t="inlineStr">
         <is>
-          <t>spume</t>
-        </is>
-      </c>
-      <c r="B21" s="6" t="inlineStr">
-        <is>
-          <t>frothy matter on liquids : foam, scum</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>ˈspyüm</t>
+          <t>querent</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="22" s="5">
       <c r="A22" s="6" t="inlineStr">
         <is>
-          <t>weft</t>
+          <t>riffled</t>
         </is>
       </c>
       <c r="B22" s="6" t="inlineStr">
         <is>
-          <t>a filling thread or yarn in weaving</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>ˈweft</t>
+          <t>to form, flow over, or move in riffles</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
+          <t>ˈri-fəl</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="23" s="5">
       <c r="A23" s="6" t="inlineStr">
         <is>
-          <t>parfleche</t>
+          <t>spume</t>
         </is>
       </c>
       <c r="B23" s="6" t="inlineStr">
         <is>
-          <t>a raw hide soaked in lye to remove the hair and dried</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>ˈpär-ˌflesh</t>
+          <t>frothy matter on liquids : foam, scum</t>
+        </is>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>ˈspyüm</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="24" s="5">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>pyrolatrous</t>
+          <t>weft</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>a filling thread or yarn in weaving</t>
+        </is>
+      </c>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>ˈweft</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="25" s="5">
       <c r="A25" s="6" t="inlineStr">
         <is>
-          <t>enhearsed</t>
+          <t>parfleche</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>a raw hide soaked in lye to remove the hair and dried</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
+        <is>
+          <t>ˈpär-ˌflesh</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="26" s="5">
       <c r="A26" s="6" t="inlineStr">
         <is>
-          <t>ideation</t>
-        </is>
-      </c>
-      <c r="B26" s="6" t="inlineStr">
-        <is>
-          <t>the capacity for or the act of forming or entertaining ideas</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>ˌī-dē-ˈā-shən</t>
+          <t>pyrolatrous</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="27" s="5">
       <c r="A27" s="6" t="inlineStr">
         <is>
-          <t>lobation</t>
-        </is>
-      </c>
-      <c r="B27" s="6" t="inlineStr">
-        <is>
-          <t>lobed</t>
+          <t>enhearsed</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="28" s="5">
       <c r="A28" s="6" t="inlineStr">
         <is>
-          <t>tatterdemalion</t>
+          <t>ideation</t>
         </is>
       </c>
       <c r="B28" s="6" t="inlineStr">
         <is>
-          <t>a person dressed in ragged clothing : ragamuffin</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>ˌta-tər-di-ˈmāl-yən</t>
+          <t>the capacity for or the act of forming or entertaining ideas</t>
+        </is>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>ˌī-dē-ˈā-shən</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="29" s="5">
       <c r="A29" s="6" t="inlineStr">
         <is>
-          <t>slalom</t>
+          <t>lobation</t>
         </is>
       </c>
       <c r="B29" s="6" t="inlineStr">
         <is>
-          <t>skiing in a zigzag or wavy course between upright obstacles (such as flags)</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>ˈslä-ləm</t>
+          <t>lobed</t>
+        </is>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>ˈlō-ˌbāt</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="30" s="5">
       <c r="A30" s="6" t="inlineStr">
         <is>
-          <t>disclets</t>
+          <t>tatterdemalion</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>a person dressed in ragged clothing : ragamuffin</t>
+        </is>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>ˌta-tər-di-ˈmāl-yən</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="31" s="5">
       <c r="A31" s="6" t="inlineStr">
         <is>
-          <t>swale</t>
+          <t>slalom</t>
         </is>
       </c>
       <c r="B31" s="6" t="inlineStr">
         <is>
-          <t>a low-lying or depressed and often wet stretch of land; also : a shallow depression on a golf course</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>ˈswāl</t>
+          <t>skiing in a zigzag or wavy course between upright obstacles (such as flags)</t>
+        </is>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>ˈslä-ləm</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="32" s="5">
       <c r="A32" s="6" t="inlineStr">
         <is>
-          <t>escarpment</t>
-        </is>
-      </c>
-      <c r="B32" s="6" t="inlineStr">
-        <is>
-          <t>a steep slope in front of a fortification</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>i-ˈskärp-mənt</t>
+          <t>disclets</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="33" s="5">
       <c r="A33" s="6" t="inlineStr">
         <is>
-          <t>kivas</t>
+          <t>swale</t>
         </is>
       </c>
       <c r="B33" s="6" t="inlineStr">
         <is>
-          <t>a Pueblo Indian ceremonial structure that is usually round and partly underground</t>
+          <t>a low-lying or depressed and often wet stretch of land; also : a shallow depression on a golf course</t>
+        </is>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>ˈswāl</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="34" s="5">
       <c r="A34" s="6" t="inlineStr">
         <is>
-          <t>euchre</t>
+          <t>escarpment</t>
         </is>
       </c>
       <c r="B34" s="6" t="inlineStr">
         <is>
-          <t>a card game in which each player is dealt five cards and the player making trump must take three tricks to win a hand</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>ˈyü-kər</t>
+          <t>a steep slope in front of a fortification</t>
+        </is>
+      </c>
+      <c r="C34" s="6" t="inlineStr">
+        <is>
+          <t>i-ˈskärp-mənt</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="35" s="5">
       <c r="A35" s="6" t="inlineStr">
         <is>
-          <t>spanceled</t>
+          <t>kivas</t>
+        </is>
+      </c>
+      <c r="B35" s="6" t="inlineStr">
+        <is>
+          <t>a Pueblo Indian ceremonial structure that is usually round and partly underground</t>
+        </is>
+      </c>
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>ˈkē-və</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="36" s="5">
       <c r="A36" s="6" t="inlineStr">
         <is>
-          <t>armature</t>
+          <t>euchre</t>
         </is>
       </c>
       <c r="B36" s="6" t="inlineStr">
         <is>
-          <t>an organ or structure (such as teeth or thorns) for offense or defense</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>ˈär-mə-ˌchu̇r</t>
+          <t>a card game in which each player is dealt five cards and the player making trump must take three tricks to win a hand</t>
+        </is>
+      </c>
+      <c r="C36" s="6" t="inlineStr">
+        <is>
+          <t>ˈyü-kər</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="37" s="5">
       <c r="A37" s="6" t="inlineStr">
         <is>
-          <t>arcature</t>
+          <t>spanceled</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="38" s="5">
       <c r="A38" s="6" t="inlineStr">
         <is>
-          <t>cravat</t>
+          <t>armature</t>
         </is>
       </c>
       <c r="B38" s="6" t="inlineStr">
         <is>
-          <t>a band or scarf worn around the neck</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>krə-ˈvat</t>
+          <t>an organ or structure (such as teeth or thorns) for offense or defense</t>
+        </is>
+      </c>
+      <c r="C38" s="6" t="inlineStr">
+        <is>
+          <t>ˈär-mə-ˌchu̇r</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="39" s="5">
       <c r="A39" s="6" t="inlineStr">
         <is>
-          <t>shoat</t>
-        </is>
-      </c>
-      <c r="B39" s="6" t="inlineStr">
-        <is>
-          <t>a young hog and especially one that has been weaned</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>ˈshōt</t>
+          <t>arcature</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="40" s="5">
       <c r="A40" s="6" t="inlineStr">
         <is>
-          <t>cartouche</t>
+          <t>cravat</t>
         </is>
       </c>
       <c r="B40" s="6" t="inlineStr">
         <is>
-          <t>a gun cartridge with a paper case</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>kär-ˈtüsh</t>
+          <t>a band or scarf worn around the neck</t>
+        </is>
+      </c>
+      <c r="C40" s="6" t="inlineStr">
+        <is>
+          <t>krə-ˈvat</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="41" s="5">
       <c r="A41" s="6" t="inlineStr">
         <is>
-          <t>debouched</t>
+          <t>shoat</t>
         </is>
       </c>
       <c r="B41" s="6" t="inlineStr">
         <is>
-          <t>to cause to emerge : discharge</t>
+          <t>a young hog and especially one that has been weaned</t>
+        </is>
+      </c>
+      <c r="C41" s="6" t="inlineStr">
+        <is>
+          <t>ˈshōt</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="42" s="5">
       <c r="A42" s="6" t="inlineStr">
         <is>
-          <t>crenellated</t>
+          <t>cartouche</t>
         </is>
       </c>
       <c r="B42" s="6" t="inlineStr">
         <is>
-          <t>having crenellations</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>ˈkre-nə-ˌlā-təd</t>
+          <t>a gun cartridge with a paper case</t>
+        </is>
+      </c>
+      <c r="C42" s="6" t="inlineStr">
+        <is>
+          <t>kär-ˈtüsh</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="43" s="5">
       <c r="A43" s="6" t="inlineStr">
         <is>
-          <t>quirting</t>
+          <t>debouched</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>to cause to emerge : discharge</t>
+        </is>
+      </c>
+      <c r="C43" s="6" t="inlineStr">
+        <is>
+          <t>di-ˈbau̇ch</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="44" s="5">
       <c r="A44" s="6" t="inlineStr">
         <is>
-          <t>argosy</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>a large ship; especially : a large merchant ship</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>ˈär-gə-sē</t>
+          <t>crenellated</t>
+        </is>
+      </c>
+      <c r="B44" s="6" t="inlineStr">
+        <is>
+          <t>having crenellations</t>
+        </is>
+      </c>
+      <c r="C44" s="6" t="inlineStr">
+        <is>
+          <t>ˈkre-nə-ˌlā-təd</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="45" s="5">
       <c r="A45" s="6" t="inlineStr">
         <is>
-          <t>sloe</t>
+          <t>argosy</t>
         </is>
       </c>
       <c r="B45" s="6" t="inlineStr">
         <is>
-          <t>the small dark globose astringent fruit of the blackthorn; also : blackthorn</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>ˈslō</t>
+          <t>a large ship; especially : a large merchant ship</t>
+        </is>
+      </c>
+      <c r="C45" s="6" t="inlineStr">
+        <is>
+          <t>ˈär-gə-sē</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="46" s="5">
       <c r="A46" s="6" t="inlineStr">
         <is>
-          <t>supernumeraries</t>
+          <t>sloe</t>
+        </is>
+      </c>
+      <c r="B46" s="6" t="inlineStr">
+        <is>
+          <t>the small dark globose astringent fruit of the blackthorn; also : blackthorn</t>
+        </is>
+      </c>
+      <c r="C46" s="6" t="inlineStr">
+        <is>
+          <t>ˈslō</t>
         </is>
       </c>
     </row>
@@ -2929,6 +2989,16 @@
           <t>caparisoned</t>
         </is>
       </c>
+      <c r="B47" s="6" t="inlineStr">
+        <is>
+          <t>to provide with or as if with a rich ornamental covering : adorn</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>kə-ˈper-ə-sən</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="48" s="5">
       <c r="A48" s="6" t="inlineStr">
@@ -2936,6 +3006,16 @@
           <t>clangorous</t>
         </is>
       </c>
+      <c r="B48" s="6" t="inlineStr">
+        <is>
+          <t>a resounding clang or medley of clangs</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ˈklaŋ-ər</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="49" s="5">
       <c r="A49" s="6" t="inlineStr">
@@ -2943,12 +3023,12 @@
           <t>pulque</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="6" t="inlineStr">
         <is>
           <t>a Mexican alcoholic beverage made from the fermented sap of various agaves (such as Agave atrovirens)</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="6" t="inlineStr">
         <is>
           <t>ˈpül-ˌkā</t>
         </is>
@@ -2960,17 +3040,19 @@
           <t>charivari</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="6" t="inlineStr">
         <is>
           <t>shivaree</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="6" t="inlineStr">
         <is>
           <t>ˌshi-və-ˈrē</t>
         </is>
       </c>
     </row>
+    <row customHeight="1" ht="12.8" r="1048575" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048576" s="5"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
@@ -2990,7 +3072,7 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.921875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.95703125" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData/>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
@@ -3011,7 +3093,7 @@
       <selection activeCell="A116" activeCellId="0" pane="topLeft" sqref="A116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.921875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.95703125" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
     <row customFormat="1" customHeight="1" ht="13.8" r="1" s="4">
       <c r="A1" s="4" t="inlineStr">

</xml_diff>

<commit_message>
added ProblemWord class to signal out nonNormal)
</commit_message>
<xml_diff>
--- a/Final/test.xlsx
+++ b/Final/test.xlsx
@@ -4,12 +4,12 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="List 1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="List 2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Mysheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="List 3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="New Title_2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
@@ -415,13 +415,11 @@
   </sheetPr>
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A8" view="normal" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A100" xSplit="0" ySplit="1"/>
-      <selection activeCell="A8" activeCellId="0" pane="topLeft" sqref="A8"/>
-      <selection activeCell="A124" activeCellId="0" pane="bottomLeft" sqref="A124"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A106" view="normal" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.95703125" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.06640625" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
     <row customFormat="1" customHeight="1" ht="13.8" r="1" s="4">
       <c r="A1" s="4" t="inlineStr">
@@ -2323,13 +2321,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A8" view="normal" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="A47" activeCellId="0" pane="topLeft" sqref="A47"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="A27" activeCellId="0" pane="topLeft" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.95703125" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.06640625" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
     <row customFormat="1" customHeight="1" ht="13.8" r="1" s="7">
       <c r="A1" s="7" t="inlineStr">
@@ -2359,7 +2357,7 @@
           <t>a riding whip with a short handle and a rawhide lash</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>ˈkwərt</t>
         </is>
@@ -2376,7 +2374,7 @@
           <t>exceeding the usual, stated, or prescribed number</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>ˌsü-pər-ˈnü-mə-ˌrer-ē</t>
         </is>
@@ -2994,7 +2992,7 @@
           <t>to provide with or as if with a rich ornamental covering : adorn</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="6" t="inlineStr">
         <is>
           <t>kə-ˈper-ə-sən</t>
         </is>
@@ -3011,7 +3009,7 @@
           <t>a resounding clang or medley of clangs</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="6" t="inlineStr">
         <is>
           <t>ˈklaŋ-ər</t>
         </is>
@@ -3046,6 +3044,23 @@
         </is>
       </c>
       <c r="C50" s="6" t="inlineStr">
+        <is>
+          <t>ˌshi-və-ˈrē</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="51" s="5">
+      <c r="A51" s="6" t="inlineStr">
+        <is>
+          <t>shivaree</t>
+        </is>
+      </c>
+      <c r="B51" s="6" t="inlineStr">
+        <is>
+          <t>a noisy mock serenade to a newly married couple</t>
+        </is>
+      </c>
+      <c r="C51" s="6" t="inlineStr">
         <is>
           <t>ˌshi-və-ˈrē</t>
         </is>
@@ -3066,14 +3081,780 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A8" view="normal" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="C10" activeCellId="0" pane="topLeft" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.95703125" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.06640625" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetData>
+    <row customFormat="1" customHeight="1" ht="13.8" r="1" s="4">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Word</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Definition</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Pronunciation</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="2" s="5">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>drubbed</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>to beat severely</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>ˈdrəb</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="3" s="5">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>catafalque</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>an ornamental structure sometimes used in funerals for the lying in state of the body</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>ˈka-tə-ˌfȯ(l)k</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="4" s="5">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>pulque</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>a Mexican alcoholic beverage made from the fermented sap of various agaves (such as Agave atrovirens)</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>ˈpül-ˌkā</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="5" s="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>ciborium</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>a goblet-shaped vessel for holding eucharistic bread</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>sə-ˈbȯr-ē-əm</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="6" s="5">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>imbreachment</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="7" s="5">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>decocted</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>to extract the flavor of by boiling</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>di-ˈkäkt</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="8" s="5">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>tiswin</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="9" s="5">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>demiculverin</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="10" s="5">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>pugmill</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="n"/>
+      <c r="C10" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="11" s="5">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>valises</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>suitcase</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>və-ˈlēs</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="12" s="5">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>holothurians</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>sea cucumber</t>
+        </is>
+      </c>
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>ˌhō-lə-ˈthu̇r-ē-ən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="13" s="5">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>nacre</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>mother-of-pearl</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>ˈnā-kər</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="14" s="5">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>littoral</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>of, relating to, or situated or growing on or near a shore especially of the sea</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>ˈli-tə-rəl</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="15" s="5">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>dunnage</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t>loose materials used to support and protect cargo in a ship's hold; also : padding in a shipping container</t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>ˈdə-nij</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="16" s="5">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>remonstrate</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>to present and urge reasons in opposition : expostulate —usually used with with</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>ˈre-mən-ˌstrāt</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="17" s="5">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>archimandrite</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>a dignitary in an Eastern church ranking below a bishop; specifically : the superior of a large monastery or group of monasteries</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="inlineStr">
+        <is>
+          <t>ˌär-kə-ˈman-ˌdrīt</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="18" s="5">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>wagontongue</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="19" s="5">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>marionettes</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>a small-scale usually wooden figure (as of a person) with jointed limbs that is moved from above by manipulation of the attached strings or wires</t>
+        </is>
+      </c>
+      <c r="C19" s="6" t="inlineStr">
+        <is>
+          <t>ˌmer-ē-ə-ˈnet</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="5">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>aslant</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>in a slanting direction : obliquely</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>ə-ˈslant</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="5">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>systole</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>a rhythmically recurrent contraction; especially : the contraction of the heart by which the blood is forced out of the chambers and into the aorta and pulmonary artery</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>ˈsi-stə-(ˌ)lē</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="5">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>scurrilous</t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>using or given to coarse language</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
+          <t>ˈskər-ə-ləs</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="5">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>siliceous</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>of, relating to, or containing silica or a silicate</t>
+        </is>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>sə-ˈli-shəs</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="5">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>groutless</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="25" s="5">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>reconnoitre</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>to make a reconnaissance of</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
+        <is>
+          <t>ˌrē-kə-ˈnȯi-tər</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="26" s="5">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>marblings</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>the action or process of making like marble especially in coloration</t>
+        </is>
+      </c>
+      <c r="C26" s="6" t="inlineStr">
+        <is>
+          <t>ˈmär-b(ə-)liŋ</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="27" s="5">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>midden</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>dunghill</t>
+        </is>
+      </c>
+      <c r="C27" s="6" t="inlineStr">
+        <is>
+          <t>ˈmi-dᵊn</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="28" s="5">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>armatures</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>an organ or structure (such as teeth or thorns) for offense or defense</t>
+        </is>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>ˈär-mə-ˌchu̇r</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="29" s="5">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>mansuete</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="30" s="5">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>attainder</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>extinction of the civil rights and capacities of a person upon sentence of death or outlawry usually after a conviction of treason</t>
+        </is>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>ə-ˈtān-dər</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="31" s="5">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>promontory</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>a high point of land or rock projecting into a body of water</t>
+        </is>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>ˈprä-mən-ˌtȯr-ē</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="32" s="5">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>esker</t>
+        </is>
+      </c>
+      <c r="B32" s="6" t="inlineStr">
+        <is>
+          <t>a long narrow ridge or mound of sand, gravel, and boulders deposited by a stream flowing on, within, or beneath a stagnant glacier</t>
+        </is>
+      </c>
+      <c r="C32" s="6" t="inlineStr">
+        <is>
+          <t>ˈe-skər</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="33" s="5">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>silica</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>the dioxide of silicon SiO2 occurring in crystalline, amorphous, and impure forms (as in quartz, opal, and sand respectively)</t>
+        </is>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>ˈsi-li-kə</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="34" s="5">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>manciple</t>
+        </is>
+      </c>
+      <c r="B34" s="6" t="inlineStr">
+        <is>
+          <t>a steward or purveyor especially for a college or monastery</t>
+        </is>
+      </c>
+      <c r="C34" s="6" t="inlineStr">
+        <is>
+          <t>ˈman(t)-sə-pəl</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="35" s="5">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>replevined</t>
+        </is>
+      </c>
+      <c r="B35" s="6" t="inlineStr">
+        <is>
+          <t>an action originating in common law and now largely codified by which a plaintiff having a right in personal property which is claimed to be wrongfully taken or detained by the defendant seeks to recover possession of the property and sometimes to obtain damages for the wrongful detention; also : a procedure allowing the plaintiff as a provisional remedy to take possession of the property prior to a judgment on the action</t>
+        </is>
+      </c>
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>ri-ˈple-vən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="36" s="5">
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>equanimity</t>
+        </is>
+      </c>
+      <c r="B36" s="6" t="inlineStr">
+        <is>
+          <t>evenness of mind especially under stress</t>
+        </is>
+      </c>
+      <c r="C36" s="6" t="inlineStr">
+        <is>
+          <t>ˌē-kwə-ˈni-mə-tē</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="37" s="5">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>emplane</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t>to board an airplane</t>
+        </is>
+      </c>
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>im-ˈplān</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="38" s="5">
+      <c r="A38" s="6" t="inlineStr">
+        <is>
+          <t>uncottered</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="39" s="5">
+      <c r="A39" s="6" t="inlineStr">
+        <is>
+          <t>sere</t>
+        </is>
+      </c>
+      <c r="B39" s="6" t="inlineStr">
+        <is>
+          <t>being dried and withered</t>
+        </is>
+      </c>
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>ˈsir</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="40" s="5">
+      <c r="A40" s="6" t="inlineStr">
+        <is>
+          <t>alcade</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="41" s="5">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>crinoline</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="inlineStr">
+        <is>
+          <t>an open-weave fabric of horsehair or cotton that is usually stiffened and used especially for interlinings and millinery</t>
+        </is>
+      </c>
+      <c r="C41" s="6" t="inlineStr">
+        <is>
+          <t>ˈkri-nə-lən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="42" s="5">
+      <c r="A42" s="6" t="inlineStr">
+        <is>
+          <t>scapegrace</t>
+        </is>
+      </c>
+      <c r="B42" s="6" t="inlineStr">
+        <is>
+          <t>an incorrigible rascal</t>
+        </is>
+      </c>
+      <c r="C42" s="6" t="inlineStr">
+        <is>
+          <t>ˈskāp-ˌgrās</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="43" s="5">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>sop</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>a piece of food dipped or steeped in a liquid</t>
+        </is>
+      </c>
+      <c r="C43" s="6" t="inlineStr">
+        <is>
+          <t>ˈsäp</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="44" s="5">
+      <c r="A44" s="6" t="inlineStr">
+        <is>
+          <t>chevron</t>
+        </is>
+      </c>
+      <c r="B44" s="6" t="inlineStr">
+        <is>
+          <t>a figure, pattern, or object having the shape of a V or an inverted V: such as</t>
+        </is>
+      </c>
+      <c r="C44" s="6" t="inlineStr">
+        <is>
+          <t>ˈshev-rən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="45" s="5">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>patrician</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>a member of one of the original citizen families of ancient Rome</t>
+        </is>
+      </c>
+      <c r="C45" s="6" t="inlineStr">
+        <is>
+          <t>pə-ˈtri-shən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="46" s="5">
+      <c r="A46" s="6" t="inlineStr">
+        <is>
+          <t>offal</t>
+        </is>
+      </c>
+      <c r="B46" s="6" t="inlineStr">
+        <is>
+          <t>the waste or by-product of a process: such as</t>
+        </is>
+      </c>
+      <c r="C46" s="6" t="inlineStr">
+        <is>
+          <t>ˈȯ-fəl</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="47" s="5">
+      <c r="A47" s="6" t="inlineStr">
+        <is>
+          <t>churlish</t>
+        </is>
+      </c>
+      <c r="B47" s="6" t="inlineStr">
+        <is>
+          <t>of, resembling, or characteristic of a churl : vulgar</t>
+        </is>
+      </c>
+      <c r="C47" s="6" t="inlineStr">
+        <is>
+          <t>ˈchər-lish</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="48" s="5">
+      <c r="A48" s="6" t="inlineStr">
+        <is>
+          <t>maudlin</t>
+        </is>
+      </c>
+      <c r="B48" s="6" t="inlineStr">
+        <is>
+          <t>drunk enough to be emotionally silly</t>
+        </is>
+      </c>
+      <c r="C48" s="6" t="inlineStr">
+        <is>
+          <t>ˈmȯd-lən</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="49" s="5">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>ignominy</t>
+        </is>
+      </c>
+      <c r="B49" s="6" t="inlineStr">
+        <is>
+          <t>deep personal humiliation and disgrace</t>
+        </is>
+      </c>
+      <c r="C49" s="6" t="inlineStr">
+        <is>
+          <t>ˈig-nə-ˌmi-nē</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="50" s="5">
+      <c r="A50" s="6" t="inlineStr">
+        <is>
+          <t>lattice</t>
+        </is>
+      </c>
+      <c r="B50" s="6" t="inlineStr">
+        <is>
+          <t>a framework or structure of crossed wood or metal strips</t>
+        </is>
+      </c>
+      <c r="C50" s="6" t="inlineStr">
+        <is>
+          <t>ˈla-təs</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="1048576" s="5"/>
+  </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
   <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
@@ -3093,7 +3874,7 @@
       <selection activeCell="A116" activeCellId="0" pane="topLeft" sqref="A116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.95703125" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.06640625" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
     <row customFormat="1" customHeight="1" ht="13.8" r="1" s="4">
       <c r="A1" s="4" t="inlineStr">

</xml_diff>